<commit_message>
Adjust some formats of the sheet
</commit_message>
<xml_diff>
--- a/Pin Assignment.xlsx
+++ b/Pin Assignment.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20343"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20351"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\University\Courses\Electronics\DigitalLogicCircuit\Experiments\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\University\Courses\MajorBasic\DigitalLogicCircuit\Experiments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A708DC0-C72A-4A9A-9836-3E5F2BF36A74}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86EF3CE2-98C2-428C-8D3D-1105F5E730D2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9756" xr2:uid="{0430B810-A713-4CED-8A03-53C7C9368B95}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="235">
   <si>
     <t>Signal Name</t>
   </si>
@@ -42,9 +42,6 @@
     <t>SW[0]</t>
   </si>
   <si>
-    <t>PIN_AB30</t>
-  </si>
-  <si>
     <t>Slide Switch[0]</t>
   </si>
   <si>
@@ -54,27 +51,18 @@
     <t>SW[1]</t>
   </si>
   <si>
-    <t>PIN_Y27</t>
-  </si>
-  <si>
     <t>Slide Switch[1]</t>
   </si>
   <si>
     <t>SW[2]</t>
   </si>
   <si>
-    <t>PIN_AB28</t>
-  </si>
-  <si>
     <t>Slide Switch[2]</t>
   </si>
   <si>
     <t>SW[3]</t>
   </si>
   <si>
-    <t>PIN_AC30</t>
-  </si>
-  <si>
     <t>Slide Switch[3]</t>
   </si>
   <si>
@@ -106,9 +94,6 @@
   </si>
   <si>
     <t>SW[7]</t>
-  </si>
-  <si>
-    <t>PIN_AD30</t>
   </si>
   <si>
     <t>Slide Switch[7]</t>
@@ -165,9 +150,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>KEY[0]</t>
-  </si>
-  <si>
     <t>PIN_AJ4</t>
   </si>
   <si>
@@ -280,9 +262,6 @@
     <t>LEDR[0]</t>
   </si>
   <si>
-    <t>PIN_AA24</t>
-  </si>
-  <si>
     <t>LED [0]</t>
   </si>
   <si>
@@ -776,6 +755,34 @@
   </si>
   <si>
     <t>Pin Assignment for DE10-Standard</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>PIN_AB28</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>KEY[0]</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>PIN_Y27</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>PIN_AB30</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>PIN_AC30</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>PIN_AD30</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>PIN_AA24</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -942,7 +949,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -955,6 +962,9 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -964,13 +974,10 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -980,6 +987,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -994,8 +1004,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1311,10 +1324,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{371CD08C-5BDA-4938-9D72-ED7CDDFF9564}">
-  <dimension ref="A1:G83"/>
+  <dimension ref="A1:G78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31:E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1329,25 +1342,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="33" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
-        <v>234</v>
-      </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
+      <c r="A1" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
     </row>
     <row r="2" spans="1:7" ht="30.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>0</v>
@@ -1363,186 +1376,186 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>37</v>
+      <c r="A3" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>32</v>
       </c>
       <c r="C3" s="10"/>
       <c r="D3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="4" spans="1:7" ht="30.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="5"/>
+      <c r="A4" s="6"/>
       <c r="B4" s="11"/>
       <c r="C4" s="12"/>
       <c r="D4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>230</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>10</v>
-      </c>
       <c r="G4" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="30.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="5"/>
+      <c r="A5" s="6"/>
       <c r="B5" s="11"/>
       <c r="C5" s="12"/>
       <c r="D5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>228</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="30.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="5"/>
+      <c r="A6" s="6"/>
       <c r="B6" s="11"/>
       <c r="C6" s="12"/>
       <c r="D6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>15</v>
+        <v>11</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>232</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="30.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="5"/>
+      <c r="A7" s="6"/>
       <c r="B7" s="11"/>
       <c r="C7" s="12"/>
       <c r="D7" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="30.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="5"/>
+      <c r="A8" s="6"/>
       <c r="B8" s="11"/>
       <c r="C8" s="12"/>
       <c r="D8" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="30.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="5"/>
+      <c r="A9" s="6"/>
       <c r="B9" s="11"/>
       <c r="C9" s="12"/>
       <c r="D9" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="5"/>
+      <c r="A10" s="6"/>
       <c r="B10" s="11"/>
       <c r="C10" s="12"/>
       <c r="D10" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>27</v>
+        <v>22</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>233</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="30.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="5"/>
+      <c r="A11" s="6"/>
       <c r="B11" s="11"/>
       <c r="C11" s="12"/>
       <c r="D11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="30.6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="6"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="G12" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="6"/>
+      <c r="B13" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F11" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="30.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="5"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="5"/>
-      <c r="B13" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="C13" s="1" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>0</v>
@@ -1558,82 +1571,82 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="5"/>
-      <c r="B14" s="8" t="s">
-        <v>66</v>
+      <c r="A14" s="6"/>
+      <c r="B14" s="9" t="s">
+        <v>60</v>
       </c>
       <c r="C14" s="10"/>
-      <c r="D14" s="2" t="s">
-        <v>39</v>
+      <c r="D14" s="4" t="s">
+        <v>229</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="5"/>
-      <c r="B15" s="7"/>
+      <c r="A15" s="6"/>
+      <c r="B15" s="18"/>
       <c r="C15" s="12"/>
       <c r="D15" s="3" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="5"/>
-      <c r="B16" s="7"/>
+      <c r="A16" s="6"/>
+      <c r="B16" s="18"/>
       <c r="C16" s="12"/>
       <c r="D16" s="2" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="5"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="13"/>
+      <c r="A17" s="6"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="14"/>
       <c r="D17" s="3" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="30.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="5"/>
+      <c r="A18" s="6"/>
       <c r="B18" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>0</v>
@@ -1649,118 +1662,118 @@
       </c>
     </row>
     <row r="19" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="5"/>
-      <c r="B19" s="8" t="s">
-        <v>67</v>
+      <c r="A19" s="6"/>
+      <c r="B19" s="9" t="s">
+        <v>61</v>
       </c>
       <c r="C19" s="10"/>
       <c r="D19" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="5"/>
+      <c r="A20" s="6"/>
       <c r="B20" s="11"/>
       <c r="C20" s="12"/>
       <c r="D20" s="3" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="5"/>
+      <c r="A21" s="6"/>
       <c r="B21" s="11"/>
       <c r="C21" s="12"/>
       <c r="D21" s="2" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="5"/>
+      <c r="A22" s="6"/>
       <c r="B22" s="11"/>
       <c r="C22" s="12"/>
       <c r="D22" s="3" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="5"/>
+      <c r="A23" s="6"/>
       <c r="B23" s="11"/>
       <c r="C23" s="12"/>
       <c r="D23" s="2" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="6"/>
-      <c r="B24" s="9"/>
-      <c r="C24" s="13"/>
+      <c r="A24" s="7"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="14"/>
       <c r="D24" s="3" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="30.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>0</v>
@@ -1776,186 +1789,186 @@
       </c>
     </row>
     <row r="26" spans="1:7" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="B26" s="8" t="s">
-        <v>69</v>
+      <c r="A26" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>63</v>
       </c>
       <c r="C26" s="10"/>
       <c r="D26" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>71</v>
+        <v>64</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>234</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="5"/>
+      <c r="A27" s="6"/>
       <c r="B27" s="11"/>
       <c r="C27" s="12"/>
       <c r="D27" s="3" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="5"/>
+      <c r="A28" s="6"/>
       <c r="B28" s="11"/>
       <c r="C28" s="12"/>
       <c r="D28" s="2" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="5"/>
+      <c r="A29" s="6"/>
       <c r="B29" s="11"/>
       <c r="C29" s="12"/>
       <c r="D29" s="3" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="5"/>
+      <c r="A30" s="6"/>
       <c r="B30" s="11"/>
       <c r="C30" s="12"/>
       <c r="D30" s="2" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="5"/>
+      <c r="A31" s="6"/>
       <c r="B31" s="11"/>
       <c r="C31" s="12"/>
       <c r="D31" s="3" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="5"/>
+      <c r="A32" s="6"/>
       <c r="B32" s="11"/>
       <c r="C32" s="12"/>
       <c r="D32" s="2" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="5"/>
+      <c r="A33" s="6"/>
       <c r="B33" s="11"/>
       <c r="C33" s="12"/>
       <c r="D33" s="3" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="5"/>
+      <c r="A34" s="6"/>
       <c r="B34" s="11"/>
       <c r="C34" s="12"/>
       <c r="D34" s="2" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="5"/>
-      <c r="B35" s="9"/>
-      <c r="C35" s="13"/>
+      <c r="A35" s="6"/>
+      <c r="B35" s="13"/>
+      <c r="C35" s="14"/>
       <c r="D35" s="3" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="5"/>
+      <c r="A36" s="6"/>
       <c r="B36" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>0</v>
@@ -1971,826 +1984,731 @@
       </c>
     </row>
     <row r="37" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="5"/>
-      <c r="B37" s="8" t="s">
+      <c r="A37" s="6"/>
+      <c r="B37" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="C37" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="6"/>
+      <c r="B38" s="11"/>
+      <c r="C38" s="16"/>
+      <c r="D38" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="6"/>
+      <c r="B39" s="11"/>
+      <c r="C39" s="16"/>
+      <c r="D39" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="C37" s="14" t="s">
+      <c r="E39" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="6"/>
+      <c r="B40" s="11"/>
+      <c r="C40" s="16"/>
+      <c r="D40" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="6"/>
+      <c r="B41" s="11"/>
+      <c r="C41" s="16"/>
+      <c r="D41" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="6"/>
+      <c r="B42" s="11"/>
+      <c r="C42" s="16"/>
+      <c r="D42" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="6"/>
+      <c r="B43" s="11"/>
+      <c r="C43" s="17"/>
+      <c r="D43" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="6"/>
+      <c r="B44" s="11"/>
+      <c r="C44" s="15" t="s">
+        <v>222</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="6"/>
+      <c r="B45" s="11"/>
+      <c r="C45" s="16"/>
+      <c r="D45" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="6"/>
+      <c r="B46" s="11"/>
+      <c r="C46" s="16"/>
+      <c r="D46" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="D37" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="G37" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="5"/>
-      <c r="B38" s="11"/>
-      <c r="C38" s="15"/>
-      <c r="D38" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="F38" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="G38" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="5"/>
-      <c r="B39" s="11"/>
-      <c r="C39" s="15"/>
-      <c r="D39" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="G39" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="5"/>
-      <c r="B40" s="11"/>
-      <c r="C40" s="15"/>
-      <c r="D40" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="E40" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="F40" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="G40" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="5"/>
-      <c r="B41" s="11"/>
-      <c r="C41" s="15"/>
-      <c r="D41" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="G41" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="5"/>
-      <c r="B42" s="11"/>
-      <c r="C42" s="15"/>
-      <c r="D42" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="E42" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="F42" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="G42" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="5"/>
-      <c r="B43" s="11"/>
-      <c r="C43" s="16"/>
-      <c r="D43" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="F43" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="G43" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="5"/>
-      <c r="B44" s="11"/>
-      <c r="C44" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G44" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="5"/>
-      <c r="B45" s="11"/>
-      <c r="C45" s="14" t="s">
-        <v>229</v>
-      </c>
-      <c r="D45" s="2" t="s">
+      <c r="E46" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="E45" s="2" t="s">
+      <c r="F46" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="F45" s="2" t="s">
+      <c r="G46" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="6"/>
+      <c r="B47" s="11"/>
+      <c r="C47" s="16"/>
+      <c r="D47" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="G45" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="5"/>
-      <c r="B46" s="11"/>
-      <c r="C46" s="15"/>
-      <c r="D46" s="3" t="s">
+      <c r="E47" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="E46" s="3" t="s">
+      <c r="F47" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="F46" s="3" t="s">
+      <c r="G47" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="6"/>
+      <c r="B48" s="11"/>
+      <c r="C48" s="16"/>
+      <c r="D48" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="G46" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="5"/>
-      <c r="B47" s="11"/>
-      <c r="C47" s="15"/>
-      <c r="D47" s="2" t="s">
+      <c r="E48" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="E47" s="2" t="s">
+      <c r="F48" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="F47" s="2" t="s">
+      <c r="G48" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="6"/>
+      <c r="B49" s="11"/>
+      <c r="C49" s="16"/>
+      <c r="D49" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="G47" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="5"/>
-      <c r="B48" s="11"/>
-      <c r="C48" s="15"/>
-      <c r="D48" s="3" t="s">
+      <c r="E49" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="E48" s="3" t="s">
+      <c r="F49" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="F48" s="3" t="s">
+      <c r="G49" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="6"/>
+      <c r="B50" s="11"/>
+      <c r="C50" s="17"/>
+      <c r="D50" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="G48" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="5"/>
-      <c r="B49" s="11"/>
-      <c r="C49" s="15"/>
-      <c r="D49" s="2" t="s">
+      <c r="E50" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="E49" s="2" t="s">
+      <c r="F50" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="F49" s="2" t="s">
+      <c r="G50" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="6"/>
+      <c r="B51" s="11"/>
+      <c r="C51" s="15" t="s">
+        <v>224</v>
+      </c>
+      <c r="D51" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="G49" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="5"/>
-      <c r="B50" s="11"/>
-      <c r="C50" s="15"/>
-      <c r="D50" s="3" t="s">
+      <c r="E51" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="E50" s="3" t="s">
+      <c r="F51" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="F50" s="3" t="s">
+      <c r="G51" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="6"/>
+      <c r="B52" s="11"/>
+      <c r="C52" s="16"/>
+      <c r="D52" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="G50" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="5"/>
-      <c r="B51" s="11"/>
-      <c r="C51" s="16"/>
-      <c r="D51" s="2" t="s">
+      <c r="E52" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="E51" s="2" t="s">
+      <c r="F52" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="F51" s="2" t="s">
+      <c r="G52" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="6"/>
+      <c r="B53" s="11"/>
+      <c r="C53" s="16"/>
+      <c r="D53" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="G51" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="5"/>
-      <c r="B52" s="11"/>
-      <c r="C52" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F52" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G52" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="5"/>
-      <c r="B53" s="11"/>
-      <c r="C53" s="14" t="s">
-        <v>231</v>
-      </c>
-      <c r="D53" s="2" t="s">
+      <c r="E53" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="E53" s="2" t="s">
+      <c r="F53" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="F53" s="2" t="s">
+      <c r="G53" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="6"/>
+      <c r="B54" s="11"/>
+      <c r="C54" s="16"/>
+      <c r="D54" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="G53" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="5"/>
-      <c r="B54" s="11"/>
-      <c r="C54" s="15"/>
-      <c r="D54" s="3" t="s">
+      <c r="E54" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="E54" s="3" t="s">
+      <c r="F54" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="F54" s="3" t="s">
+      <c r="G54" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="6"/>
+      <c r="B55" s="11"/>
+      <c r="C55" s="16"/>
+      <c r="D55" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="G54" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="5"/>
-      <c r="B55" s="11"/>
-      <c r="C55" s="15"/>
-      <c r="D55" s="2" t="s">
+      <c r="E55" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="E55" s="2" t="s">
+      <c r="F55" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="F55" s="2" t="s">
+      <c r="G55" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="6"/>
+      <c r="B56" s="11"/>
+      <c r="C56" s="16"/>
+      <c r="D56" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="G55" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="5"/>
-      <c r="B56" s="11"/>
-      <c r="C56" s="15"/>
-      <c r="D56" s="3" t="s">
+      <c r="E56" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="E56" s="3" t="s">
+      <c r="F56" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="F56" s="3" t="s">
+      <c r="G56" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="6"/>
+      <c r="B57" s="11"/>
+      <c r="C57" s="17"/>
+      <c r="D57" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="G56" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="5"/>
-      <c r="B57" s="11"/>
-      <c r="C57" s="15"/>
-      <c r="D57" s="2" t="s">
+      <c r="E57" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="E57" s="2" t="s">
+      <c r="F57" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="F57" s="2" t="s">
+      <c r="G57" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="6"/>
+      <c r="B58" s="11"/>
+      <c r="C58" s="15" t="s">
+        <v>223</v>
+      </c>
+      <c r="D58" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="G57" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="5"/>
-      <c r="B58" s="11"/>
-      <c r="C58" s="15"/>
-      <c r="D58" s="3" t="s">
+      <c r="E58" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="E58" s="3" t="s">
+      <c r="F58" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="F58" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="G58" s="3" t="s">
-        <v>42</v>
+      <c r="G58" s="2" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="5"/>
+      <c r="A59" s="6"/>
       <c r="B59" s="11"/>
       <c r="C59" s="16"/>
-      <c r="D59" s="2" t="s">
+      <c r="D59" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="E59" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="E59" s="2" t="s">
+      <c r="F59" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="F59" s="2" t="s">
+      <c r="G59" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="6"/>
+      <c r="B60" s="11"/>
+      <c r="C60" s="16"/>
+      <c r="D60" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="G59" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="5"/>
-      <c r="B60" s="11"/>
-      <c r="C60" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F60" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G60" s="1" t="s">
-        <v>3</v>
+      <c r="E60" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="G60" s="2" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="5"/>
+      <c r="A61" s="6"/>
       <c r="B61" s="11"/>
-      <c r="C61" s="14" t="s">
-        <v>230</v>
-      </c>
-      <c r="D61" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="E61" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="F61" s="2" t="s">
+      <c r="C61" s="16"/>
+      <c r="D61" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="G61" s="2" t="s">
-        <v>42</v>
+      <c r="E61" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="F61" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="G61" s="3" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="62" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="5"/>
+      <c r="A62" s="6"/>
       <c r="B62" s="11"/>
-      <c r="C62" s="15"/>
-      <c r="D62" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="E62" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="F62" s="3" t="s">
+      <c r="C62" s="16"/>
+      <c r="D62" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="G62" s="3" t="s">
-        <v>42</v>
+      <c r="E62" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="G62" s="2" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="5"/>
+      <c r="A63" s="6"/>
       <c r="B63" s="11"/>
-      <c r="C63" s="15"/>
-      <c r="D63" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="E63" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="F63" s="2" t="s">
+      <c r="C63" s="16"/>
+      <c r="D63" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="G63" s="2" t="s">
-        <v>42</v>
+      <c r="E63" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="F63" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="G63" s="3" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="64" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="5"/>
+      <c r="A64" s="6"/>
       <c r="B64" s="11"/>
-      <c r="C64" s="15"/>
-      <c r="D64" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="E64" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="F64" s="3" t="s">
+      <c r="C64" s="17"/>
+      <c r="D64" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="G64" s="3" t="s">
-        <v>42</v>
+      <c r="E64" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="G64" s="2" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="5"/>
+      <c r="A65" s="6"/>
       <c r="B65" s="11"/>
-      <c r="C65" s="15"/>
+      <c r="C65" s="15" t="s">
+        <v>225</v>
+      </c>
       <c r="D65" s="2" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="G65" s="2" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="66" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="5"/>
+      <c r="A66" s="6"/>
       <c r="B66" s="11"/>
-      <c r="C66" s="15"/>
+      <c r="C66" s="16"/>
       <c r="D66" s="3" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="G66" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="5"/>
+      <c r="A67" s="6"/>
       <c r="B67" s="11"/>
       <c r="C67" s="16"/>
       <c r="D67" s="2" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="G67" s="2" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="68" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="5"/>
+      <c r="A68" s="6"/>
       <c r="B68" s="11"/>
-      <c r="C68" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E68" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F68" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G68" s="1" t="s">
-        <v>3</v>
+      <c r="C68" s="16"/>
+      <c r="D68" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="E68" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="F68" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="G68" s="3" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="5"/>
+      <c r="A69" s="6"/>
       <c r="B69" s="11"/>
-      <c r="C69" s="14" t="s">
-        <v>232</v>
-      </c>
+      <c r="C69" s="16"/>
       <c r="D69" s="2" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="G69" s="2" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="5"/>
+      <c r="A70" s="6"/>
       <c r="B70" s="11"/>
-      <c r="C70" s="15"/>
+      <c r="C70" s="16"/>
       <c r="D70" s="3" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="F70" s="3" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="G70" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="5"/>
+      <c r="A71" s="6"/>
       <c r="B71" s="11"/>
-      <c r="C71" s="15"/>
+      <c r="C71" s="17"/>
       <c r="D71" s="2" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="G71" s="2" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="5"/>
+      <c r="A72" s="6"/>
       <c r="B72" s="11"/>
-      <c r="C72" s="15"/>
-      <c r="D72" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="E72" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="F72" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="G72" s="3" t="s">
-        <v>42</v>
+      <c r="C72" s="15" t="s">
+        <v>226</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="F72" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="G72" s="2" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="5"/>
+      <c r="A73" s="6"/>
       <c r="B73" s="11"/>
-      <c r="C73" s="15"/>
-      <c r="D73" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="E73" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="F73" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="G73" s="2" t="s">
-        <v>42</v>
+      <c r="C73" s="16"/>
+      <c r="D73" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="E73" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="F73" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="G73" s="3" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="74" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="5"/>
+      <c r="A74" s="6"/>
       <c r="B74" s="11"/>
-      <c r="C74" s="15"/>
-      <c r="D74" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="E74" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="F74" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="G74" s="3" t="s">
-        <v>42</v>
+      <c r="C74" s="16"/>
+      <c r="D74" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="F74" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="G74" s="2" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="5"/>
+      <c r="A75" s="6"/>
       <c r="B75" s="11"/>
       <c r="C75" s="16"/>
-      <c r="D75" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="E75" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="F75" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="G75" s="2" t="s">
-        <v>42</v>
+      <c r="D75" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="E75" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="F75" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="G75" s="3" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="5"/>
+      <c r="A76" s="6"/>
       <c r="B76" s="11"/>
-      <c r="C76" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E76" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F76" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G76" s="1" t="s">
-        <v>3</v>
+      <c r="C76" s="16"/>
+      <c r="D76" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="F76" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="G76" s="2" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="77" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="5"/>
+      <c r="A77" s="6"/>
       <c r="B77" s="11"/>
-      <c r="C77" s="14" t="s">
-        <v>233</v>
-      </c>
-      <c r="D77" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="E77" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="F77" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="G77" s="2" t="s">
-        <v>42</v>
+      <c r="C77" s="16"/>
+      <c r="D77" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="E77" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="F77" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="G77" s="3" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="78" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="5"/>
+      <c r="A78" s="6"/>
       <c r="B78" s="11"/>
-      <c r="C78" s="15"/>
-      <c r="D78" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="E78" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="F78" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="G78" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="5"/>
-      <c r="B79" s="11"/>
-      <c r="C79" s="15"/>
-      <c r="D79" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="E79" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="F79" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="G79" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="5"/>
-      <c r="B80" s="11"/>
-      <c r="C80" s="15"/>
-      <c r="D80" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="E80" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="F80" s="3" t="s">
+      <c r="C78" s="17"/>
+      <c r="D78" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="G80" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="5"/>
-      <c r="B81" s="11"/>
-      <c r="C81" s="15"/>
-      <c r="D81" s="2" t="s">
+      <c r="E78" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="E81" s="2" t="s">
+      <c r="F78" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="F81" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="G81" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="5"/>
-      <c r="B82" s="11"/>
-      <c r="C82" s="15"/>
-      <c r="D82" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="E82" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="F82" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="G82" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="5"/>
-      <c r="B83" s="11"/>
-      <c r="C83" s="16"/>
-      <c r="D83" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="E83" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="F83" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="G83" s="2" t="s">
-        <v>42</v>
+      <c r="G78" s="2" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -2798,15 +2716,15 @@
     <mergeCell ref="A3:A24"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="B19:C24"/>
-    <mergeCell ref="A26:A83"/>
+    <mergeCell ref="A26:A78"/>
     <mergeCell ref="B26:C35"/>
-    <mergeCell ref="B37:B83"/>
+    <mergeCell ref="B37:B78"/>
     <mergeCell ref="C37:C43"/>
-    <mergeCell ref="C45:C51"/>
-    <mergeCell ref="C53:C59"/>
-    <mergeCell ref="C61:C67"/>
-    <mergeCell ref="C69:C75"/>
-    <mergeCell ref="C77:C83"/>
+    <mergeCell ref="C44:C50"/>
+    <mergeCell ref="C51:C57"/>
+    <mergeCell ref="C58:C64"/>
+    <mergeCell ref="C65:C71"/>
+    <mergeCell ref="C72:C78"/>
     <mergeCell ref="B3:C12"/>
     <mergeCell ref="B14:C17"/>
   </mergeCells>

</xml_diff>

<commit_message>
Upgrade xlsx: Add PS/2 Serial Port
</commit_message>
<xml_diff>
--- a/Pin Assignment.xlsx
+++ b/Pin Assignment.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20351"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\University\Courses\MajorBasic\DigitalLogicCircuit\Experiments\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DLCExp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86EF3CE2-98C2-428C-8D3D-1105F5E730D2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9756" xr2:uid="{0430B810-A713-4CED-8A03-53C7C9368B95}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9750"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="248">
   <si>
     <t>Signal Name</t>
   </si>
@@ -42,6 +41,9 @@
     <t>SW[0]</t>
   </si>
   <si>
+    <t>PIN_AB30</t>
+  </si>
+  <si>
     <t>Slide Switch[0]</t>
   </si>
   <si>
@@ -51,18 +53,27 @@
     <t>SW[1]</t>
   </si>
   <si>
+    <t>PIN_Y27</t>
+  </si>
+  <si>
     <t>Slide Switch[1]</t>
   </si>
   <si>
     <t>SW[2]</t>
   </si>
   <si>
+    <t>PIN_AB28</t>
+  </si>
+  <si>
     <t>Slide Switch[2]</t>
   </si>
   <si>
     <t>SW[3]</t>
   </si>
   <si>
+    <t>PIN_AC30</t>
+  </si>
+  <si>
     <t>Slide Switch[3]</t>
   </si>
   <si>
@@ -94,6 +105,9 @@
   </si>
   <si>
     <t>SW[7]</t>
+  </si>
+  <si>
+    <t>PIN_AD30</t>
   </si>
   <si>
     <t>Slide Switch[7]</t>
@@ -150,6 +164,9 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
+    <t>KEY[0]</t>
+  </si>
+  <si>
     <t>PIN_AJ4</t>
   </si>
   <si>
@@ -262,6 +279,9 @@
     <t>LEDR[0]</t>
   </si>
   <si>
+    <t>PIN_AA24</t>
+  </si>
+  <si>
     <t>LED [0]</t>
   </si>
   <si>
@@ -350,9 +370,6 @@
   </si>
   <si>
     <t>HEX0[0]</t>
-  </si>
-  <si>
-    <t>PIN_W17</t>
   </si>
   <si>
     <t>Seven Segment Digit 0[0]</t>
@@ -758,39 +775,74 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>PIN_AB28</t>
+    <t>PIN_W17</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>KEY[0]</t>
+    <r>
+      <rPr>
+        <sz val="13.75"/>
+        <color rgb="FF24292E"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>键盘</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.75"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> PS/2 Serial Port (PS2)</t>
+    </r>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>PIN_Y27</t>
+    <t>PS2_CLK</t>
+  </si>
+  <si>
+    <t>PS2_DAT</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>PIN_AB30</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>PIN_AC30</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>PIN_AD30</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>PIN_AA24</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <t>PS2_CLK2</t>
+  </si>
+  <si>
+    <t>PS2_DAT2</t>
+  </si>
+  <si>
+    <t>PIN_AB25</t>
+  </si>
+  <si>
+    <t>PIN_AA25</t>
+  </si>
+  <si>
+    <t>PIN_AC25</t>
+  </si>
+  <si>
+    <t>PIN_AB26</t>
+  </si>
+  <si>
+    <t>PS/2 Clock</t>
+  </si>
+  <si>
+    <t>PS/2 Data</t>
+  </si>
+  <si>
+    <t>PS/2 Clock (reserved for second PS/2 device)</t>
+  </si>
+  <si>
+    <t>PS/2 Data (reserved for second PS/2 device)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -849,6 +901,13 @@
       <color theme="1"/>
       <name val="Segoe UI"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="13.75"/>
+      <color rgb="FF24292E"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="4">
@@ -949,7 +1008,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1006,9 +1065,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1323,27 +1379,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{371CD08C-5BDA-4938-9D72-ED7CDDFF9564}">
-  <dimension ref="A1:G78"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31:E35"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.77734375" customWidth="1"/>
-    <col min="2" max="2" width="12.21875" customWidth="1"/>
-    <col min="4" max="4" width="14.88671875" customWidth="1"/>
-    <col min="5" max="5" width="9.44140625" customWidth="1"/>
+    <col min="1" max="1" width="12.75" customWidth="1"/>
+    <col min="2" max="2" width="12.25" customWidth="1"/>
+    <col min="4" max="4" width="14.875" customWidth="1"/>
+    <col min="5" max="5" width="9.5" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
-    <col min="7" max="7" width="9.77734375" customWidth="1"/>
-    <col min="12" max="13" width="8.88671875" customWidth="1"/>
+    <col min="7" max="7" width="9.75" customWidth="1"/>
+    <col min="12" max="13" width="8.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="33" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="33.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
@@ -1352,15 +1408,15 @@
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
     </row>
-    <row r="2" spans="1:7" ht="30.6" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>0</v>
@@ -1375,187 +1431,187 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C3" s="10"/>
       <c r="D3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>231</v>
+      <c r="E3" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="30.6" thickBot="1" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
       <c r="B4" s="11"/>
       <c r="C4" s="12"/>
       <c r="D4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="19" t="s">
-        <v>230</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="30.6" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:7" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
       <c r="B5" s="11"/>
       <c r="C5" s="12"/>
       <c r="D5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>228</v>
+        <v>11</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="30.6" thickBot="1" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
       <c r="B6" s="11"/>
       <c r="C6" s="12"/>
       <c r="D6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="19" t="s">
-        <v>232</v>
+        <v>14</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="30.6" thickBot="1" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="11"/>
       <c r="C7" s="12"/>
       <c r="D7" s="2" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="30.6" thickBot="1" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
       <c r="B8" s="11"/>
       <c r="C8" s="12"/>
       <c r="D8" s="3" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="30.6" thickBot="1" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="11"/>
       <c r="C9" s="12"/>
       <c r="D9" s="2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="30.6" thickBot="1" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
       <c r="B10" s="11"/>
       <c r="C10" s="12"/>
       <c r="D10" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10" s="19" t="s">
-        <v>233</v>
+        <v>26</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="30.6" thickBot="1" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="11"/>
       <c r="C11" s="12"/>
       <c r="D11" s="2" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="30.6" thickBot="1" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="13"/>
       <c r="C12" s="14"/>
       <c r="D12" s="3" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>0</v>
@@ -1570,83 +1626,83 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="9" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="C14" s="10"/>
-      <c r="D14" s="4" t="s">
-        <v>229</v>
+      <c r="D14" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
       <c r="B15" s="18"/>
       <c r="C15" s="12"/>
       <c r="D15" s="3" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="18"/>
       <c r="C16" s="12"/>
       <c r="D16" s="2" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
       <c r="B17" s="13"/>
       <c r="C17" s="14"/>
       <c r="D17" s="3" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="30.6" thickBot="1" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>0</v>
@@ -1661,1072 +1717,1143 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="9" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="C19" s="10"/>
       <c r="D19" s="2" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
       <c r="B20" s="11"/>
       <c r="C20" s="12"/>
       <c r="D20" s="3" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
       <c r="B21" s="11"/>
       <c r="C21" s="12"/>
       <c r="D21" s="2" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6"/>
       <c r="B22" s="11"/>
       <c r="C22" s="12"/>
       <c r="D22" s="3" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="E22" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F22" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F22" s="3" t="s">
-        <v>48</v>
-      </c>
       <c r="G22" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
       <c r="B23" s="11"/>
       <c r="C23" s="12"/>
       <c r="D23" s="2" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="7"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="6"/>
       <c r="B24" s="13"/>
       <c r="C24" s="14"/>
       <c r="D24" s="3" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="30.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="B26" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="C26" s="10"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="35.450000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="6"/>
+      <c r="B25" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="C25" s="10"/>
+      <c r="D25" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="35.450000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="6"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="12"/>
       <c r="D26" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>234</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>237</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="6"/>
       <c r="B27" s="11"/>
       <c r="C27" s="12"/>
-      <c r="D27" s="3" t="s">
-        <v>66</v>
+      <c r="D27" s="2" t="s">
+        <v>238</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>67</v>
+        <v>242</v>
       </c>
       <c r="F27" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="7"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="14"/>
+      <c r="D28" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="G27" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="6"/>
-      <c r="B28" s="11"/>
-      <c r="C28" s="12"/>
-      <c r="D28" s="2" t="s">
+      <c r="B30" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="C30" s="10"/>
+      <c r="D30" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="F28" s="2" t="s">
+      <c r="E30" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="G28" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="6"/>
-      <c r="B29" s="11"/>
-      <c r="C29" s="12"/>
-      <c r="D29" s="3" t="s">
+      <c r="F30" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="E29" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="G29" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="6"/>
-      <c r="B30" s="11"/>
-      <c r="C30" s="12"/>
-      <c r="D30" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>77</v>
-      </c>
       <c r="G30" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="6"/>
       <c r="B31" s="11"/>
       <c r="C31" s="12"/>
       <c r="D31" s="3" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="6"/>
       <c r="B32" s="11"/>
       <c r="C32" s="12"/>
       <c r="D32" s="2" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="6"/>
       <c r="B33" s="11"/>
       <c r="C33" s="12"/>
       <c r="D33" s="3" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="6"/>
       <c r="B34" s="11"/>
       <c r="C34" s="12"/>
       <c r="D34" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="6"/>
+      <c r="B35" s="11"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F35" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="E34" s="2" t="s">
+      <c r="G35" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="6"/>
+      <c r="B36" s="11"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="F34" s="2" t="s">
+      <c r="E36" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="G34" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="6"/>
-      <c r="B35" s="13"/>
-      <c r="C35" s="14"/>
-      <c r="D35" s="3" t="s">
+      <c r="F36" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="E35" s="3" t="s">
+      <c r="G36" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="6"/>
+      <c r="B37" s="11"/>
+      <c r="C37" s="12"/>
+      <c r="D37" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="F35" s="3" t="s">
+      <c r="E37" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="G35" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="6"/>
-      <c r="B36" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="6"/>
-      <c r="B37" s="9" t="s">
+      <c r="F37" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="C37" s="15" t="s">
-        <v>115</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="G37" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G37" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="6"/>
       <c r="B38" s="11"/>
-      <c r="C38" s="16"/>
-      <c r="D38" s="3" t="s">
+      <c r="C38" s="12"/>
+      <c r="D38" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="6"/>
+      <c r="B39" s="13"/>
+      <c r="C39" s="14"/>
+      <c r="D39" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="E38" s="3" t="s">
+      <c r="E39" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="F38" s="3" t="s">
+      <c r="F39" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="G38" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="6"/>
-      <c r="B39" s="11"/>
-      <c r="C39" s="16"/>
-      <c r="D39" s="2" t="s">
+      <c r="G39" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="6"/>
+      <c r="B40" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="6"/>
+      <c r="B41" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="E39" s="2" t="s">
+      <c r="C41" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="D41" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="F39" s="2" t="s">
+      <c r="E41" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="F41" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="G39" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="6"/>
-      <c r="B40" s="11"/>
-      <c r="C40" s="16"/>
-      <c r="D40" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="E40" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="F40" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="G40" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="6"/>
-      <c r="B41" s="11"/>
-      <c r="C41" s="16"/>
-      <c r="D41" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>108</v>
-      </c>
       <c r="G41" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="6"/>
       <c r="B42" s="11"/>
       <c r="C42" s="16"/>
       <c r="D42" s="3" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="6"/>
       <c r="B43" s="11"/>
-      <c r="C43" s="17"/>
+      <c r="C43" s="16"/>
       <c r="D43" s="2" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="6"/>
       <c r="B44" s="11"/>
-      <c r="C44" s="15" t="s">
-        <v>222</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="F44" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="G44" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C44" s="16"/>
+      <c r="D44" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="6"/>
       <c r="B45" s="11"/>
       <c r="C45" s="16"/>
-      <c r="D45" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="E45" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="F45" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="G45" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D45" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A46" s="6"/>
       <c r="B46" s="11"/>
       <c r="C46" s="16"/>
-      <c r="D46" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="F46" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="G46" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D46" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A47" s="6"/>
       <c r="B47" s="11"/>
-      <c r="C47" s="16"/>
-      <c r="D47" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="E47" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="F47" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="G47" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C47" s="17"/>
+      <c r="D47" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A48" s="6"/>
       <c r="B48" s="11"/>
-      <c r="C48" s="16"/>
+      <c r="C48" s="15" t="s">
+        <v>228</v>
+      </c>
       <c r="D48" s="2" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="6"/>
       <c r="B49" s="11"/>
       <c r="C49" s="16"/>
       <c r="D49" s="3" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A50" s="6"/>
       <c r="B50" s="11"/>
-      <c r="C50" s="17"/>
+      <c r="C50" s="16"/>
       <c r="D50" s="2" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A51" s="6"/>
       <c r="B51" s="11"/>
-      <c r="C51" s="15" t="s">
-        <v>224</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="F51" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="G51" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C51" s="16"/>
+      <c r="D51" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="F51" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="G51" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A52" s="6"/>
       <c r="B52" s="11"/>
       <c r="C52" s="16"/>
-      <c r="D52" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="E52" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="F52" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="G52" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D52" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="G52" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A53" s="6"/>
       <c r="B53" s="11"/>
       <c r="C53" s="16"/>
-      <c r="D53" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="F53" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="G53" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D53" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="F53" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="G53" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A54" s="6"/>
       <c r="B54" s="11"/>
-      <c r="C54" s="16"/>
-      <c r="D54" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="E54" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="F54" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="G54" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C54" s="17"/>
+      <c r="D54" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A55" s="6"/>
       <c r="B55" s="11"/>
-      <c r="C55" s="16"/>
+      <c r="C55" s="15" t="s">
+        <v>230</v>
+      </c>
       <c r="D55" s="2" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A56" s="6"/>
       <c r="B56" s="11"/>
       <c r="C56" s="16"/>
       <c r="D56" s="3" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A57" s="6"/>
       <c r="B57" s="11"/>
-      <c r="C57" s="17"/>
+      <c r="C57" s="16"/>
       <c r="D57" s="2" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A58" s="6"/>
       <c r="B58" s="11"/>
-      <c r="C58" s="15" t="s">
-        <v>223</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="E58" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="F58" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="G58" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C58" s="16"/>
+      <c r="D58" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="F58" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="G58" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A59" s="6"/>
       <c r="B59" s="11"/>
       <c r="C59" s="16"/>
-      <c r="D59" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="E59" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="F59" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="G59" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D59" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="G59" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A60" s="6"/>
       <c r="B60" s="11"/>
       <c r="C60" s="16"/>
-      <c r="D60" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="E60" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="F60" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="G60" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D60" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="F60" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="G60" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A61" s="6"/>
       <c r="B61" s="11"/>
-      <c r="C61" s="16"/>
-      <c r="D61" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="E61" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="F61" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="G61" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C61" s="17"/>
+      <c r="D61" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G61" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A62" s="6"/>
       <c r="B62" s="11"/>
-      <c r="C62" s="16"/>
+      <c r="C62" s="15" t="s">
+        <v>229</v>
+      </c>
       <c r="D62" s="2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A63" s="6"/>
       <c r="B63" s="11"/>
       <c r="C63" s="16"/>
       <c r="D63" s="3" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="G63" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A64" s="6"/>
       <c r="B64" s="11"/>
-      <c r="C64" s="17"/>
+      <c r="C64" s="16"/>
       <c r="D64" s="2" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A65" s="6"/>
       <c r="B65" s="11"/>
-      <c r="C65" s="15" t="s">
-        <v>225</v>
-      </c>
-      <c r="D65" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="E65" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="F65" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="G65" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C65" s="16"/>
+      <c r="D65" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="F65" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="G65" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A66" s="6"/>
       <c r="B66" s="11"/>
       <c r="C66" s="16"/>
-      <c r="D66" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="E66" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="F66" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="G66" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D66" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="F66" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="G66" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A67" s="6"/>
       <c r="B67" s="11"/>
       <c r="C67" s="16"/>
-      <c r="D67" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="E67" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="F67" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="G67" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D67" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="E67" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="F67" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="G67" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A68" s="6"/>
       <c r="B68" s="11"/>
-      <c r="C68" s="16"/>
-      <c r="D68" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="E68" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="F68" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="G68" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C68" s="17"/>
+      <c r="D68" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="F68" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="G68" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A69" s="6"/>
       <c r="B69" s="11"/>
-      <c r="C69" s="16"/>
+      <c r="C69" s="15" t="s">
+        <v>231</v>
+      </c>
       <c r="D69" s="2" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="G69" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A70" s="6"/>
       <c r="B70" s="11"/>
       <c r="C70" s="16"/>
       <c r="D70" s="3" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="F70" s="3" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="G70" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A71" s="6"/>
       <c r="B71" s="11"/>
-      <c r="C71" s="17"/>
+      <c r="C71" s="16"/>
       <c r="D71" s="2" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="G71" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A72" s="6"/>
       <c r="B72" s="11"/>
-      <c r="C72" s="15" t="s">
-        <v>226</v>
-      </c>
-      <c r="D72" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="E72" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="F72" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="G72" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C72" s="16"/>
+      <c r="D72" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E72" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="F72" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="G72" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A73" s="6"/>
       <c r="B73" s="11"/>
       <c r="C73" s="16"/>
-      <c r="D73" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="E73" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="F73" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="G73" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D73" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="F73" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="G73" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A74" s="6"/>
       <c r="B74" s="11"/>
       <c r="C74" s="16"/>
-      <c r="D74" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="E74" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="F74" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="G74" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D74" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="E74" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="F74" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="G74" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A75" s="6"/>
       <c r="B75" s="11"/>
-      <c r="C75" s="16"/>
-      <c r="D75" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="E75" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="F75" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="G75" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C75" s="17"/>
+      <c r="D75" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="F75" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="G75" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A76" s="6"/>
       <c r="B76" s="11"/>
-      <c r="C76" s="16"/>
+      <c r="C76" s="15" t="s">
+        <v>232</v>
+      </c>
       <c r="D76" s="2" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="G76" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A77" s="6"/>
       <c r="B77" s="11"/>
       <c r="C77" s="16"/>
       <c r="D77" s="3" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="F77" s="3" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="G77" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A78" s="6"/>
       <c r="B78" s="11"/>
-      <c r="C78" s="17"/>
+      <c r="C78" s="16"/>
       <c r="D78" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="F78" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="G78" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="6"/>
+      <c r="B79" s="11"/>
+      <c r="C79" s="16"/>
+      <c r="D79" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="E79" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="F79" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="G79" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="6"/>
+      <c r="B80" s="11"/>
+      <c r="C80" s="16"/>
+      <c r="D80" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="E78" s="2" t="s">
+      <c r="E80" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="F78" s="2" t="s">
+      <c r="F80" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="G78" s="2" t="s">
-        <v>36</v>
+      <c r="G80" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="6"/>
+      <c r="B81" s="11"/>
+      <c r="C81" s="16"/>
+      <c r="D81" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="E81" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="F81" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="G81" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="6"/>
+      <c r="B82" s="11"/>
+      <c r="C82" s="17"/>
+      <c r="D82" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="F82" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="G82" s="2" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="A3:A24"/>
+  <mergeCells count="15">
+    <mergeCell ref="B25:C28"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="B19:C24"/>
-    <mergeCell ref="A26:A78"/>
-    <mergeCell ref="B26:C35"/>
-    <mergeCell ref="B37:B78"/>
-    <mergeCell ref="C37:C43"/>
-    <mergeCell ref="C44:C50"/>
-    <mergeCell ref="C51:C57"/>
-    <mergeCell ref="C58:C64"/>
-    <mergeCell ref="C65:C71"/>
-    <mergeCell ref="C72:C78"/>
+    <mergeCell ref="A30:A82"/>
+    <mergeCell ref="B30:C39"/>
+    <mergeCell ref="B41:B82"/>
+    <mergeCell ref="C41:C47"/>
+    <mergeCell ref="C48:C54"/>
+    <mergeCell ref="C55:C61"/>
+    <mergeCell ref="C62:C68"/>
+    <mergeCell ref="C69:C75"/>
+    <mergeCell ref="C76:C82"/>
     <mergeCell ref="B3:C12"/>
     <mergeCell ref="B14:C17"/>
+    <mergeCell ref="A3:A28"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update .xlsx: Fix some formats
</commit_message>
<xml_diff>
--- a/Pin Assignment.xlsx
+++ b/Pin Assignment.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="248">
   <si>
     <t>Signal Name</t>
   </si>
@@ -779,6 +779,43 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
+    <t>PS2_CLK</t>
+  </si>
+  <si>
+    <t>PS2_DAT</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>PS2_CLK2</t>
+  </si>
+  <si>
+    <t>PS2_DAT2</t>
+  </si>
+  <si>
+    <t>PIN_AB25</t>
+  </si>
+  <si>
+    <t>PIN_AA25</t>
+  </si>
+  <si>
+    <t>PIN_AC25</t>
+  </si>
+  <si>
+    <t>PIN_AB26</t>
+  </si>
+  <si>
+    <t>PS/2 Clock</t>
+  </si>
+  <si>
+    <t>PS/2 Data</t>
+  </si>
+  <si>
+    <t>PS/2 Clock (reserved for second PS/2 device)</t>
+  </si>
+  <si>
+    <t>PS/2 Data (reserved for second PS/2 device)</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="13.75"/>
@@ -799,43 +836,6 @@
       <t xml:space="preserve"> PS/2 Serial Port (PS2)</t>
     </r>
     <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>PS2_CLK</t>
-  </si>
-  <si>
-    <t>PS2_DAT</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>PS2_CLK2</t>
-  </si>
-  <si>
-    <t>PS2_DAT2</t>
-  </si>
-  <si>
-    <t>PIN_AB25</t>
-  </si>
-  <si>
-    <t>PIN_AA25</t>
-  </si>
-  <si>
-    <t>PIN_AC25</t>
-  </si>
-  <si>
-    <t>PIN_AB26</t>
-  </si>
-  <si>
-    <t>PS/2 Clock</t>
-  </si>
-  <si>
-    <t>PS/2 Data</t>
-  </si>
-  <si>
-    <t>PS/2 Clock (reserved for second PS/2 device)</t>
-  </si>
-  <si>
-    <t>PS/2 Data (reserved for second PS/2 device)</t>
   </si>
 </sst>
 </file>
@@ -1024,18 +1024,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1054,6 +1042,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1064,6 +1061,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1380,10 +1380,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G82"/>
+  <dimension ref="A1:G83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1398,15 +1398,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="33.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="11" t="s">
         <v>233</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
     </row>
     <row r="2" spans="1:7" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1432,13 +1432,13 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="10"/>
+      <c r="C3" s="6"/>
       <c r="D3" s="2" t="s">
         <v>4</v>
       </c>
@@ -1453,9 +1453,9 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="12"/>
+      <c r="A4" s="13"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="8"/>
       <c r="D4" s="3" t="s">
         <v>8</v>
       </c>
@@ -1470,9 +1470,9 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="12"/>
+      <c r="A5" s="13"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="8"/>
       <c r="D5" s="2" t="s">
         <v>11</v>
       </c>
@@ -1487,9 +1487,9 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="12"/>
+      <c r="A6" s="13"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="8"/>
       <c r="D6" s="3" t="s">
         <v>14</v>
       </c>
@@ -1504,9 +1504,9 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="12"/>
+      <c r="A7" s="13"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="8"/>
       <c r="D7" s="2" t="s">
         <v>17</v>
       </c>
@@ -1521,9 +1521,9 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="12"/>
+      <c r="A8" s="13"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="8"/>
       <c r="D8" s="3" t="s">
         <v>20</v>
       </c>
@@ -1538,9 +1538,9 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="12"/>
+      <c r="A9" s="13"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="8"/>
       <c r="D9" s="2" t="s">
         <v>23</v>
       </c>
@@ -1555,9 +1555,9 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="12"/>
+      <c r="A10" s="13"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="8"/>
       <c r="D10" s="3" t="s">
         <v>26</v>
       </c>
@@ -1572,9 +1572,9 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="12"/>
+      <c r="A11" s="13"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="8"/>
       <c r="D11" s="2" t="s">
         <v>29</v>
       </c>
@@ -1589,9 +1589,9 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="14"/>
+      <c r="A12" s="13"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="10"/>
       <c r="D12" s="3" t="s">
         <v>32</v>
       </c>
@@ -1606,7 +1606,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
+      <c r="A13" s="13"/>
       <c r="B13" s="1" t="s">
         <v>35</v>
       </c>
@@ -1627,11 +1627,11 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="6"/>
-      <c r="B14" s="9" t="s">
+      <c r="A14" s="13"/>
+      <c r="B14" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="C14" s="10"/>
+      <c r="C14" s="6"/>
       <c r="D14" s="2" t="s">
         <v>39</v>
       </c>
@@ -1646,9 +1646,9 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="6"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="12"/>
+      <c r="A15" s="13"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="8"/>
       <c r="D15" s="3" t="s">
         <v>43</v>
       </c>
@@ -1663,9 +1663,9 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="12"/>
+      <c r="A16" s="13"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="8"/>
       <c r="D16" s="2" t="s">
         <v>46</v>
       </c>
@@ -1680,9 +1680,9 @@
       </c>
     </row>
     <row r="17" spans="1:7" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="6"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="14"/>
+      <c r="A17" s="13"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="10"/>
       <c r="D17" s="3" t="s">
         <v>49</v>
       </c>
@@ -1697,7 +1697,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
+      <c r="A18" s="13"/>
       <c r="B18" s="1" t="s">
         <v>35</v>
       </c>
@@ -1718,11 +1718,11 @@
       </c>
     </row>
     <row r="19" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
-      <c r="B19" s="9" t="s">
+      <c r="A19" s="13"/>
+      <c r="B19" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="C19" s="10"/>
+      <c r="C19" s="6"/>
       <c r="D19" s="2" t="s">
         <v>52</v>
       </c>
@@ -1737,9 +1737,9 @@
       </c>
     </row>
     <row r="20" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="6"/>
-      <c r="B20" s="11"/>
-      <c r="C20" s="12"/>
+      <c r="A20" s="13"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="8"/>
       <c r="D20" s="3" t="s">
         <v>55</v>
       </c>
@@ -1754,9 +1754,9 @@
       </c>
     </row>
     <row r="21" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="6"/>
-      <c r="B21" s="11"/>
-      <c r="C21" s="12"/>
+      <c r="A21" s="13"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="8"/>
       <c r="D21" s="2" t="s">
         <v>57</v>
       </c>
@@ -1771,9 +1771,9 @@
       </c>
     </row>
     <row r="22" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="6"/>
-      <c r="B22" s="11"/>
-      <c r="C22" s="12"/>
+      <c r="A22" s="13"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="8"/>
       <c r="D22" s="3" t="s">
         <v>59</v>
       </c>
@@ -1788,9 +1788,9 @@
       </c>
     </row>
     <row r="23" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="6"/>
-      <c r="B23" s="11"/>
-      <c r="C23" s="12"/>
+      <c r="A23" s="13"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="8"/>
       <c r="D23" s="2" t="s">
         <v>61</v>
       </c>
@@ -1805,9 +1805,9 @@
       </c>
     </row>
     <row r="24" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="6"/>
-      <c r="B24" s="13"/>
-      <c r="C24" s="14"/>
+      <c r="A24" s="13"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="10"/>
       <c r="D24" s="3" t="s">
         <v>64</v>
       </c>
@@ -1821,1039 +1821,1060 @@
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="35.450000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="6"/>
-      <c r="B25" s="9" t="s">
+    <row r="25" spans="1:7" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="13"/>
+      <c r="B25" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="35.450000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="13"/>
+      <c r="B26" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="C26" s="6"/>
+      <c r="D26" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="C25" s="10"/>
-      <c r="D25" s="2" t="s">
+      <c r="E26" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="35.450000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="13"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="E25" s="3" t="s">
+      <c r="E27" s="3" t="s">
         <v>240</v>
       </c>
-      <c r="F25" s="3" t="s">
+      <c r="F27" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="G25" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="35.450000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="6"/>
-      <c r="B26" s="11"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="2" t="s">
+      <c r="G27" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="13"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="E28" s="3" t="s">
         <v>241</v>
       </c>
-      <c r="F26" s="3" t="s">
+      <c r="F28" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="G26" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="6"/>
-      <c r="B27" s="11"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="2" t="s">
+      <c r="G28" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="18"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="E27" s="3" t="s">
+      <c r="E29" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="F27" s="3" t="s">
+      <c r="F29" s="3" t="s">
         <v>246</v>
       </c>
-      <c r="G27" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="7"/>
-      <c r="B28" s="13"/>
-      <c r="C28" s="14"/>
-      <c r="D28" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>243</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>247</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
+      <c r="G29" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B30" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C30" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="D30" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="E30" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F29" s="1" t="s">
+      <c r="F30" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G29" s="1" t="s">
+      <c r="G30" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
+    <row r="31" spans="1:7" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="B30" s="9" t="s">
+      <c r="B31" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="C30" s="10"/>
-      <c r="D30" s="2" t="s">
+      <c r="C31" s="6"/>
+      <c r="D31" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E30" s="2" t="s">
+      <c r="E31" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="F30" s="2" t="s">
+      <c r="F31" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="G30" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="6"/>
-      <c r="B31" s="11"/>
-      <c r="C31" s="12"/>
-      <c r="D31" s="3" t="s">
+      <c r="G31" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="13"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="E31" s="3" t="s">
+      <c r="E32" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="F31" s="3" t="s">
+      <c r="F32" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="G31" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="6"/>
-      <c r="B32" s="11"/>
-      <c r="C32" s="12"/>
-      <c r="D32" s="2" t="s">
+      <c r="G32" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="13"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="E32" s="2" t="s">
+      <c r="E33" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="F32" s="2" t="s">
+      <c r="F33" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="G32" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="6"/>
-      <c r="B33" s="11"/>
-      <c r="C33" s="12"/>
-      <c r="D33" s="3" t="s">
+      <c r="G33" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="13"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="E33" s="3" t="s">
+      <c r="E34" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="F33" s="3" t="s">
+      <c r="F34" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="G33" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="6"/>
-      <c r="B34" s="11"/>
-      <c r="C34" s="12"/>
-      <c r="D34" s="2" t="s">
+      <c r="G34" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="13"/>
+      <c r="B35" s="7"/>
+      <c r="C35" s="8"/>
+      <c r="D35" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="E34" s="2" t="s">
+      <c r="E35" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="F34" s="2" t="s">
+      <c r="F35" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="G34" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="6"/>
-      <c r="B35" s="11"/>
-      <c r="C35" s="12"/>
-      <c r="D35" s="3" t="s">
+      <c r="G35" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="13"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="E35" s="3" t="s">
+      <c r="E36" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="F35" s="3" t="s">
+      <c r="F36" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="G35" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="6"/>
-      <c r="B36" s="11"/>
-      <c r="C36" s="12"/>
-      <c r="D36" s="2" t="s">
+      <c r="G36" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="13"/>
+      <c r="B37" s="7"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="E36" s="2" t="s">
+      <c r="E37" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="F36" s="2" t="s">
+      <c r="F37" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="G36" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="6"/>
-      <c r="B37" s="11"/>
-      <c r="C37" s="12"/>
-      <c r="D37" s="3" t="s">
+      <c r="G37" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="13"/>
+      <c r="B38" s="7"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="E37" s="3" t="s">
+      <c r="E38" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="F37" s="3" t="s">
+      <c r="F38" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="G37" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="6"/>
-      <c r="B38" s="11"/>
-      <c r="C38" s="12"/>
-      <c r="D38" s="2" t="s">
+      <c r="G38" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="13"/>
+      <c r="B39" s="7"/>
+      <c r="C39" s="8"/>
+      <c r="D39" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="E38" s="2" t="s">
+      <c r="E39" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="F38" s="2" t="s">
+      <c r="F39" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="G38" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="6"/>
-      <c r="B39" s="13"/>
-      <c r="C39" s="14"/>
-      <c r="D39" s="3" t="s">
+      <c r="G39" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="13"/>
+      <c r="B40" s="9"/>
+      <c r="C40" s="10"/>
+      <c r="D40" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="E39" s="3" t="s">
+      <c r="E40" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="F39" s="3" t="s">
+      <c r="F40" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="G39" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="6"/>
-      <c r="B40" s="1" t="s">
+      <c r="G40" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="13"/>
+      <c r="B41" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C41" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="D40" s="1" t="s">
+      <c r="D41" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E40" s="1" t="s">
+      <c r="E41" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F40" s="1" t="s">
+      <c r="F41" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G40" s="1" t="s">
+      <c r="G41" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="6"/>
-      <c r="B41" s="9" t="s">
+    <row r="42" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="13"/>
+      <c r="B42" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="C41" s="15" t="s">
+      <c r="C42" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="D42" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="E41" s="4" t="s">
+      <c r="E42" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="F41" s="2" t="s">
+      <c r="F42" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="G41" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="6"/>
-      <c r="B42" s="11"/>
-      <c r="C42" s="16"/>
-      <c r="D42" s="3" t="s">
+      <c r="G42" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="13"/>
+      <c r="B43" s="7"/>
+      <c r="C43" s="15"/>
+      <c r="D43" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="E42" s="3" t="s">
+      <c r="E43" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="F42" s="3" t="s">
+      <c r="F43" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="G42" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="6"/>
-      <c r="B43" s="11"/>
-      <c r="C43" s="16"/>
-      <c r="D43" s="2" t="s">
+      <c r="G43" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="13"/>
+      <c r="B44" s="7"/>
+      <c r="C44" s="15"/>
+      <c r="D44" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="E43" s="2" t="s">
+      <c r="E44" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="F43" s="2" t="s">
+      <c r="F44" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="G43" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="6"/>
-      <c r="B44" s="11"/>
-      <c r="C44" s="16"/>
-      <c r="D44" s="3" t="s">
+      <c r="G44" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="13"/>
+      <c r="B45" s="7"/>
+      <c r="C45" s="15"/>
+      <c r="D45" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="E44" s="3" t="s">
+      <c r="E45" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="F44" s="3" t="s">
+      <c r="F45" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="G44" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="6"/>
-      <c r="B45" s="11"/>
-      <c r="C45" s="16"/>
-      <c r="D45" s="2" t="s">
+      <c r="G45" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="13"/>
+      <c r="B46" s="7"/>
+      <c r="C46" s="15"/>
+      <c r="D46" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="E45" s="2" t="s">
+      <c r="E46" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="F45" s="2" t="s">
+      <c r="F46" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="G45" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="6"/>
-      <c r="B46" s="11"/>
-      <c r="C46" s="16"/>
-      <c r="D46" s="3" t="s">
+      <c r="G46" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="13"/>
+      <c r="B47" s="7"/>
+      <c r="C47" s="15"/>
+      <c r="D47" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="E46" s="3" t="s">
+      <c r="E47" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="F46" s="3" t="s">
+      <c r="F47" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="G46" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="6"/>
-      <c r="B47" s="11"/>
-      <c r="C47" s="17"/>
-      <c r="D47" s="2" t="s">
+      <c r="G47" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="13"/>
+      <c r="B48" s="7"/>
+      <c r="C48" s="16"/>
+      <c r="D48" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="E47" s="2" t="s">
+      <c r="E48" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="F47" s="2" t="s">
+      <c r="F48" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="G47" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="6"/>
-      <c r="B48" s="11"/>
-      <c r="C48" s="15" t="s">
+      <c r="G48" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="13"/>
+      <c r="B49" s="7"/>
+      <c r="C49" s="14" t="s">
         <v>228</v>
       </c>
-      <c r="D48" s="2" t="s">
+      <c r="D49" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="E48" s="2" t="s">
+      <c r="E49" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="F48" s="2" t="s">
+      <c r="F49" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="G48" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="6"/>
-      <c r="B49" s="11"/>
-      <c r="C49" s="16"/>
-      <c r="D49" s="3" t="s">
+      <c r="G49" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="13"/>
+      <c r="B50" s="7"/>
+      <c r="C50" s="15"/>
+      <c r="D50" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="E49" s="3" t="s">
+      <c r="E50" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="F49" s="3" t="s">
+      <c r="F50" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="G49" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="6"/>
-      <c r="B50" s="11"/>
-      <c r="C50" s="16"/>
-      <c r="D50" s="2" t="s">
+      <c r="G50" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="13"/>
+      <c r="B51" s="7"/>
+      <c r="C51" s="15"/>
+      <c r="D51" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="E50" s="2" t="s">
+      <c r="E51" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="F50" s="2" t="s">
+      <c r="F51" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="G50" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="6"/>
-      <c r="B51" s="11"/>
-      <c r="C51" s="16"/>
-      <c r="D51" s="3" t="s">
+      <c r="G51" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="13"/>
+      <c r="B52" s="7"/>
+      <c r="C52" s="15"/>
+      <c r="D52" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="E51" s="3" t="s">
+      <c r="E52" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="F51" s="3" t="s">
+      <c r="F52" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="G51" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="6"/>
-      <c r="B52" s="11"/>
-      <c r="C52" s="16"/>
-      <c r="D52" s="2" t="s">
+      <c r="G52" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="13"/>
+      <c r="B53" s="7"/>
+      <c r="C53" s="15"/>
+      <c r="D53" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="E52" s="2" t="s">
+      <c r="E53" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="F52" s="2" t="s">
+      <c r="F53" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="G52" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="6"/>
-      <c r="B53" s="11"/>
-      <c r="C53" s="16"/>
-      <c r="D53" s="3" t="s">
+      <c r="G53" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="13"/>
+      <c r="B54" s="7"/>
+      <c r="C54" s="15"/>
+      <c r="D54" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="E53" s="3" t="s">
+      <c r="E54" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="F53" s="3" t="s">
+      <c r="F54" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="G53" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="6"/>
-      <c r="B54" s="11"/>
-      <c r="C54" s="17"/>
-      <c r="D54" s="2" t="s">
+      <c r="G54" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="13"/>
+      <c r="B55" s="7"/>
+      <c r="C55" s="16"/>
+      <c r="D55" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="E54" s="2" t="s">
+      <c r="E55" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="F54" s="2" t="s">
+      <c r="F55" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="G54" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="6"/>
-      <c r="B55" s="11"/>
-      <c r="C55" s="15" t="s">
+      <c r="G55" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="13"/>
+      <c r="B56" s="7"/>
+      <c r="C56" s="14" t="s">
         <v>230</v>
       </c>
-      <c r="D55" s="2" t="s">
+      <c r="D56" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="E55" s="2" t="s">
+      <c r="E56" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="F55" s="2" t="s">
+      <c r="F56" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="G55" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="6"/>
-      <c r="B56" s="11"/>
-      <c r="C56" s="16"/>
-      <c r="D56" s="3" t="s">
+      <c r="G56" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="13"/>
+      <c r="B57" s="7"/>
+      <c r="C57" s="15"/>
+      <c r="D57" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="E56" s="3" t="s">
+      <c r="E57" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="F56" s="3" t="s">
+      <c r="F57" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="G56" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="6"/>
-      <c r="B57" s="11"/>
-      <c r="C57" s="16"/>
-      <c r="D57" s="2" t="s">
+      <c r="G57" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="13"/>
+      <c r="B58" s="7"/>
+      <c r="C58" s="15"/>
+      <c r="D58" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="E57" s="2" t="s">
+      <c r="E58" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="F57" s="2" t="s">
+      <c r="F58" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="G57" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="6"/>
-      <c r="B58" s="11"/>
-      <c r="C58" s="16"/>
-      <c r="D58" s="3" t="s">
+      <c r="G58" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="13"/>
+      <c r="B59" s="7"/>
+      <c r="C59" s="15"/>
+      <c r="D59" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="E58" s="3" t="s">
+      <c r="E59" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="F58" s="3" t="s">
+      <c r="F59" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="G58" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="6"/>
-      <c r="B59" s="11"/>
-      <c r="C59" s="16"/>
-      <c r="D59" s="2" t="s">
+      <c r="G59" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="13"/>
+      <c r="B60" s="7"/>
+      <c r="C60" s="15"/>
+      <c r="D60" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="E59" s="2" t="s">
+      <c r="E60" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="F59" s="2" t="s">
+      <c r="F60" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="G59" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="6"/>
-      <c r="B60" s="11"/>
-      <c r="C60" s="16"/>
-      <c r="D60" s="3" t="s">
+      <c r="G60" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="13"/>
+      <c r="B61" s="7"/>
+      <c r="C61" s="15"/>
+      <c r="D61" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="E60" s="3" t="s">
+      <c r="E61" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="F60" s="3" t="s">
+      <c r="F61" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="G60" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="6"/>
-      <c r="B61" s="11"/>
-      <c r="C61" s="17"/>
-      <c r="D61" s="2" t="s">
+      <c r="G61" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="13"/>
+      <c r="B62" s="7"/>
+      <c r="C62" s="16"/>
+      <c r="D62" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="E61" s="2" t="s">
+      <c r="E62" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="F61" s="2" t="s">
+      <c r="F62" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="G61" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="6"/>
-      <c r="B62" s="11"/>
-      <c r="C62" s="15" t="s">
+      <c r="G62" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="13"/>
+      <c r="B63" s="7"/>
+      <c r="C63" s="14" t="s">
         <v>229</v>
       </c>
-      <c r="D62" s="2" t="s">
+      <c r="D63" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="E62" s="2" t="s">
+      <c r="E63" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="F62" s="2" t="s">
+      <c r="F63" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="G62" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="6"/>
-      <c r="B63" s="11"/>
-      <c r="C63" s="16"/>
-      <c r="D63" s="3" t="s">
+      <c r="G63" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="13"/>
+      <c r="B64" s="7"/>
+      <c r="C64" s="15"/>
+      <c r="D64" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="E63" s="3" t="s">
+      <c r="E64" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="F63" s="3" t="s">
+      <c r="F64" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="G63" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="6"/>
-      <c r="B64" s="11"/>
-      <c r="C64" s="16"/>
-      <c r="D64" s="2" t="s">
+      <c r="G64" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="13"/>
+      <c r="B65" s="7"/>
+      <c r="C65" s="15"/>
+      <c r="D65" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="E64" s="2" t="s">
+      <c r="E65" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="F64" s="2" t="s">
+      <c r="F65" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="G64" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="6"/>
-      <c r="B65" s="11"/>
-      <c r="C65" s="16"/>
-      <c r="D65" s="3" t="s">
+      <c r="G65" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="13"/>
+      <c r="B66" s="7"/>
+      <c r="C66" s="15"/>
+      <c r="D66" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="E65" s="3" t="s">
+      <c r="E66" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="F65" s="3" t="s">
+      <c r="F66" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="G65" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="6"/>
-      <c r="B66" s="11"/>
-      <c r="C66" s="16"/>
-      <c r="D66" s="2" t="s">
+      <c r="G66" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="13"/>
+      <c r="B67" s="7"/>
+      <c r="C67" s="15"/>
+      <c r="D67" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="E66" s="2" t="s">
+      <c r="E67" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="F66" s="2" t="s">
+      <c r="F67" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="G66" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="6"/>
-      <c r="B67" s="11"/>
-      <c r="C67" s="16"/>
-      <c r="D67" s="3" t="s">
+      <c r="G67" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="13"/>
+      <c r="B68" s="7"/>
+      <c r="C68" s="15"/>
+      <c r="D68" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="E67" s="3" t="s">
+      <c r="E68" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="F67" s="3" t="s">
+      <c r="F68" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="G67" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="6"/>
-      <c r="B68" s="11"/>
-      <c r="C68" s="17"/>
-      <c r="D68" s="2" t="s">
+      <c r="G68" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="13"/>
+      <c r="B69" s="7"/>
+      <c r="C69" s="16"/>
+      <c r="D69" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="E68" s="2" t="s">
+      <c r="E69" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="F68" s="2" t="s">
+      <c r="F69" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="G68" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="6"/>
-      <c r="B69" s="11"/>
-      <c r="C69" s="15" t="s">
+      <c r="G69" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="13"/>
+      <c r="B70" s="7"/>
+      <c r="C70" s="14" t="s">
         <v>231</v>
       </c>
-      <c r="D69" s="2" t="s">
+      <c r="D70" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="E69" s="2" t="s">
+      <c r="E70" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="F69" s="2" t="s">
+      <c r="F70" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="G69" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="6"/>
-      <c r="B70" s="11"/>
-      <c r="C70" s="16"/>
-      <c r="D70" s="3" t="s">
+      <c r="G70" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="13"/>
+      <c r="B71" s="7"/>
+      <c r="C71" s="15"/>
+      <c r="D71" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="E70" s="3" t="s">
+      <c r="E71" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="F70" s="3" t="s">
+      <c r="F71" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="G70" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="6"/>
-      <c r="B71" s="11"/>
-      <c r="C71" s="16"/>
-      <c r="D71" s="2" t="s">
+      <c r="G71" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="13"/>
+      <c r="B72" s="7"/>
+      <c r="C72" s="15"/>
+      <c r="D72" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="E71" s="2" t="s">
+      <c r="E72" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="F71" s="2" t="s">
+      <c r="F72" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="G71" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="6"/>
-      <c r="B72" s="11"/>
-      <c r="C72" s="16"/>
-      <c r="D72" s="3" t="s">
+      <c r="G72" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="13"/>
+      <c r="B73" s="7"/>
+      <c r="C73" s="15"/>
+      <c r="D73" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="E72" s="3" t="s">
+      <c r="E73" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="F72" s="3" t="s">
+      <c r="F73" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="G72" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="6"/>
-      <c r="B73" s="11"/>
-      <c r="C73" s="16"/>
-      <c r="D73" s="2" t="s">
+      <c r="G73" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="13"/>
+      <c r="B74" s="7"/>
+      <c r="C74" s="15"/>
+      <c r="D74" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="E73" s="2" t="s">
+      <c r="E74" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="F73" s="2" t="s">
+      <c r="F74" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="G73" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="6"/>
-      <c r="B74" s="11"/>
-      <c r="C74" s="16"/>
-      <c r="D74" s="3" t="s">
+      <c r="G74" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="13"/>
+      <c r="B75" s="7"/>
+      <c r="C75" s="15"/>
+      <c r="D75" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="E74" s="3" t="s">
+      <c r="E75" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="F74" s="3" t="s">
+      <c r="F75" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="G74" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="6"/>
-      <c r="B75" s="11"/>
-      <c r="C75" s="17"/>
-      <c r="D75" s="2" t="s">
+      <c r="G75" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="13"/>
+      <c r="B76" s="7"/>
+      <c r="C76" s="16"/>
+      <c r="D76" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="E75" s="2" t="s">
+      <c r="E76" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="F75" s="2" t="s">
+      <c r="F76" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="G75" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="6"/>
-      <c r="B76" s="11"/>
-      <c r="C76" s="15" t="s">
+      <c r="G76" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="13"/>
+      <c r="B77" s="7"/>
+      <c r="C77" s="14" t="s">
         <v>232</v>
       </c>
-      <c r="D76" s="2" t="s">
+      <c r="D77" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="E76" s="2" t="s">
+      <c r="E77" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="F76" s="2" t="s">
+      <c r="F77" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="G76" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="6"/>
-      <c r="B77" s="11"/>
-      <c r="C77" s="16"/>
-      <c r="D77" s="3" t="s">
+      <c r="G77" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="13"/>
+      <c r="B78" s="7"/>
+      <c r="C78" s="15"/>
+      <c r="D78" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="E77" s="3" t="s">
+      <c r="E78" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="F77" s="3" t="s">
+      <c r="F78" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="G77" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="6"/>
-      <c r="B78" s="11"/>
-      <c r="C78" s="16"/>
-      <c r="D78" s="2" t="s">
+      <c r="G78" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="13"/>
+      <c r="B79" s="7"/>
+      <c r="C79" s="15"/>
+      <c r="D79" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="E78" s="2" t="s">
+      <c r="E79" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="F78" s="2" t="s">
+      <c r="F79" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="G78" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="6"/>
-      <c r="B79" s="11"/>
-      <c r="C79" s="16"/>
-      <c r="D79" s="3" t="s">
+      <c r="G79" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="13"/>
+      <c r="B80" s="7"/>
+      <c r="C80" s="15"/>
+      <c r="D80" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="E79" s="3" t="s">
+      <c r="E80" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="F79" s="3" t="s">
+      <c r="F80" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="G79" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="6"/>
-      <c r="B80" s="11"/>
-      <c r="C80" s="16"/>
-      <c r="D80" s="2" t="s">
+      <c r="G80" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="13"/>
+      <c r="B81" s="7"/>
+      <c r="C81" s="15"/>
+      <c r="D81" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="E80" s="2" t="s">
+      <c r="E81" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="F80" s="2" t="s">
+      <c r="F81" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="G80" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="6"/>
-      <c r="B81" s="11"/>
-      <c r="C81" s="16"/>
-      <c r="D81" s="3" t="s">
+      <c r="G81" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="13"/>
+      <c r="B82" s="7"/>
+      <c r="C82" s="15"/>
+      <c r="D82" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="E81" s="3" t="s">
+      <c r="E82" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="F81" s="3" t="s">
+      <c r="F82" s="3" t="s">
         <v>223</v>
       </c>
-      <c r="G81" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="6"/>
-      <c r="B82" s="11"/>
-      <c r="C82" s="17"/>
-      <c r="D82" s="2" t="s">
+      <c r="G82" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="13"/>
+      <c r="B83" s="7"/>
+      <c r="C83" s="16"/>
+      <c r="D83" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="E82" s="2" t="s">
+      <c r="E83" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="F82" s="2" t="s">
+      <c r="F83" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="G82" s="2" t="s">
+      <c r="G83" s="2" t="s">
         <v>42</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B25:C28"/>
+    <mergeCell ref="B26:C29"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="B19:C24"/>
-    <mergeCell ref="A30:A82"/>
-    <mergeCell ref="B30:C39"/>
-    <mergeCell ref="B41:B82"/>
-    <mergeCell ref="C41:C47"/>
-    <mergeCell ref="C48:C54"/>
-    <mergeCell ref="C55:C61"/>
-    <mergeCell ref="C62:C68"/>
-    <mergeCell ref="C69:C75"/>
-    <mergeCell ref="C76:C82"/>
+    <mergeCell ref="A31:A83"/>
+    <mergeCell ref="B31:C40"/>
+    <mergeCell ref="B42:B83"/>
+    <mergeCell ref="C42:C48"/>
+    <mergeCell ref="C49:C55"/>
+    <mergeCell ref="C56:C62"/>
+    <mergeCell ref="C63:C69"/>
+    <mergeCell ref="C70:C76"/>
+    <mergeCell ref="C77:C83"/>
     <mergeCell ref="B3:C12"/>
     <mergeCell ref="B14:C17"/>
-    <mergeCell ref="A3:A28"/>
+    <mergeCell ref="A3:A29"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>